<commit_message>
Multi Isothermal Translate OK
</commit_message>
<xml_diff>
--- a/Dados/NaCl_dados_entrada_teste_MI.xlsx
+++ b/Dados/NaCl_dados_entrada_teste_MI.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/KATHERINE/JAFOS/Artigo JAFO5/Dados/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marce\Desktop\Salt_Solubility_MS\Dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2466086B-D445-AD4B-AE66-18FDD265EE26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9EAE8B0-2831-4F6F-BB3C-6E30CCDC8A49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1740" yWindow="0" windowWidth="23260" windowHeight="16540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2610" yWindow="-13620" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="parametros" sheetId="1" r:id="rId1"/>
-    <sheet name="dados" sheetId="2" r:id="rId2"/>
+    <sheet name="Parameter" sheetId="1" r:id="rId1"/>
+    <sheet name="Data" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -52,9 +52,6 @@
     <t>T (K)</t>
   </si>
   <si>
-    <t>Massa molar sal (g/mol)</t>
-  </si>
-  <si>
     <t>Beta0_ref_25C</t>
   </si>
   <si>
@@ -79,31 +76,34 @@
     <t>Monteiro(2021)</t>
   </si>
   <si>
-    <t>Parametro</t>
-  </si>
-  <si>
-    <t>ParamValor</t>
-  </si>
-  <si>
-    <t>DeltaG transf (J/mol)</t>
-  </si>
-  <si>
-    <t>Raio cation</t>
-  </si>
-  <si>
-    <t>Raio anion</t>
-  </si>
-  <si>
-    <t>Carga cation</t>
-  </si>
-  <si>
-    <t>Carga anion</t>
-  </si>
-  <si>
-    <t>Coef esteq cation</t>
-  </si>
-  <si>
-    <t>Coef esteq anion</t>
+    <t>Parameter</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Cation radius</t>
+  </si>
+  <si>
+    <t>Anion radius</t>
+  </si>
+  <si>
+    <t>Cation charge</t>
+  </si>
+  <si>
+    <t>Anion Charge</t>
+  </si>
+  <si>
+    <t>Cation stoichiometric coefficient</t>
+  </si>
+  <si>
+    <t>Anion stoichiometric coefficient</t>
+  </si>
+  <si>
+    <t>Salt Molar Mass (g/mol)</t>
+  </si>
+  <si>
+    <t>Transf DeltaG (J/mol)</t>
   </si>
 </sst>
 </file>
@@ -566,135 +566,135 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.1640625" style="1"/>
-    <col min="4" max="5" width="9.1640625" style="2"/>
-    <col min="6" max="6" width="10.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.1640625" style="3"/>
+    <col min="1" max="1" width="30.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="1"/>
+    <col min="4" max="5" width="9.140625" style="2"/>
+    <col min="6" max="6" width="10.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="3"/>
     <col min="8" max="8" width="15" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.1640625" style="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B4" s="5">
         <v>2.1800000000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B5" s="5">
         <v>2.2400000000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B6" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B7" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B8" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B9" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="B10" s="5">
         <v>58.442999999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B11" s="5">
         <v>7000</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B12" s="11"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B13" s="7">
         <v>7.6499999999999999E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B14" s="7">
         <v>0.26640000000000003</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B15" s="7">
         <v>1.2700000000000001E-3</v>
@@ -703,6 +703,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -710,25 +711,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A58" sqref="A58"/>
+    <sheetView topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.1640625" style="13" customWidth="1"/>
-    <col min="2" max="2" width="16.1640625" style="13" customWidth="1"/>
-    <col min="3" max="3" width="13.1640625" style="13" customWidth="1"/>
+    <col min="1" max="1" width="15.140625" style="13" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" style="13" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" style="13" customWidth="1"/>
     <col min="4" max="4" width="20" style="13" customWidth="1"/>
-    <col min="5" max="16384" width="9.1640625" style="12"/>
+    <col min="5" max="16384" width="9.140625" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C1" s="9" t="s">
         <v>2</v>
@@ -737,7 +738,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="14">
         <v>293.14999999999998</v>
       </c>
@@ -748,10 +749,10 @@
         <v>0.26400000000000001</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="14">
         <v>293.14999999999998</v>
       </c>
@@ -762,10 +763,10 @@
         <v>0.25259999999999999</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="14">
         <v>293.14999999999998</v>
       </c>
@@ -776,10 +777,10 @@
         <v>0.2422</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="14">
         <v>293.14999999999998</v>
       </c>
@@ -790,10 +791,10 @@
         <v>0.2298</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="14">
         <v>293.14999999999998</v>
       </c>
@@ -804,10 +805,10 @@
         <v>0.21829999999999999</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="14">
         <v>293.14999999999998</v>
       </c>
@@ -818,10 +819,10 @@
         <v>0.19489999999999999</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="14">
         <v>293.14999999999998</v>
       </c>
@@ -832,10 +833,10 @@
         <v>0.1731</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="14">
         <v>293.14999999999998</v>
       </c>
@@ -846,10 +847,10 @@
         <v>0.15140000000000001</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="14">
         <v>293.14999999999998</v>
       </c>
@@ -860,10 +861,10 @@
         <v>0.12989999999999999</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="14">
         <v>293.14999999999998</v>
       </c>
@@ -874,10 +875,10 @@
         <v>0.1113</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="14">
         <v>293.14999999999998</v>
       </c>
@@ -888,10 +889,10 @@
         <v>9.3399999999999997E-2</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="14">
         <v>293.14999999999998</v>
       </c>
@@ -902,10 +903,10 @@
         <v>7.6399999999999996E-2</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="14">
         <v>293.14999999999998</v>
       </c>
@@ -916,10 +917,10 @@
         <v>7.3400000000000007E-2</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="14">
         <v>293.14999999999998</v>
       </c>
@@ -930,10 +931,10 @@
         <v>6.6600000000000006E-2</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="14">
         <v>318.14999999999998</v>
       </c>
@@ -944,10 +945,10 @@
         <v>0.26840000000000003</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="14">
         <v>318.14999999999998</v>
       </c>
@@ -958,10 +959,10 @@
         <v>0.24629999999999999</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="14">
         <v>318.14999999999998</v>
       </c>
@@ -972,10 +973,10 @@
         <v>0.22209999999999999</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="14">
         <v>318.14999999999998</v>
       </c>
@@ -986,10 +987,10 @@
         <v>0.20100000000000001</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="14">
         <v>318.14999999999998</v>
       </c>
@@ -1000,10 +1001,10 @@
         <v>0.1789</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="14">
         <v>318.14999999999998</v>
       </c>
@@ -1014,10 +1015,10 @@
         <v>0.156</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="14">
         <v>318.14999999999998</v>
       </c>
@@ -1028,10 +1029,10 @@
         <v>0.13350000000000001</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="14">
         <v>318.14999999999998</v>
       </c>
@@ -1042,10 +1043,10 @@
         <v>0.1137</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="14">
         <v>318.14999999999998</v>
       </c>
@@ -1056,10 +1057,10 @@
         <v>9.6000000000000002E-2</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="14">
         <v>318.14999999999998</v>
       </c>
@@ -1070,10 +1071,10 @@
         <v>7.85E-2</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="14">
         <v>318.14999999999998</v>
       </c>
@@ -1084,10 +1085,10 @@
         <v>7.2700000000000001E-2</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="14">
         <v>318.14999999999998</v>
       </c>
@@ -1098,10 +1099,10 @@
         <v>6.6000000000000003E-2</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="14">
         <v>348.15</v>
       </c>
@@ -1112,10 +1113,10 @@
         <v>0.27510000000000001</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="14">
         <v>348.15</v>
       </c>
@@ -1126,10 +1127,10 @@
         <v>0.253</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="14">
         <v>348.15</v>
       </c>
@@ -1140,10 +1141,10 @@
         <v>0.23019999999999999</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="14">
         <v>348.15</v>
       </c>
@@ -1154,10 +1155,10 @@
         <v>0.20599999999999999</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="14">
         <v>348.15</v>
       </c>
@@ -1168,10 +1169,10 @@
         <v>0.184</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="14">
         <v>348.15</v>
       </c>
@@ -1182,10 +1183,10 @@
         <v>0.16059999999999999</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="14">
         <v>348.15</v>
       </c>
@@ -1196,10 +1197,10 @@
         <v>0.1386</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="14">
         <v>348.15</v>
       </c>
@@ -1210,10 +1211,10 @@
         <v>0.1173</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="14">
         <v>348.15</v>
       </c>
@@ -1224,10 +1225,10 @@
         <v>9.7100000000000006E-2</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="14">
         <v>348.15</v>
       </c>
@@ -1238,10 +1239,10 @@
         <v>7.9699999999999993E-2</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="14">
         <v>348.15</v>
       </c>
@@ -1252,10 +1253,10 @@
         <v>7.1999999999999995E-2</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="14">
         <v>348.15</v>
       </c>
@@ -1266,10 +1267,10 @@
         <v>6.4699999999999994E-2</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="14">
         <v>363.15</v>
       </c>
@@ -1280,10 +1281,10 @@
         <v>0.27879999999999999</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="14">
         <v>363.15</v>
       </c>
@@ -1294,10 +1295,10 @@
         <v>0.25629999999999997</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="14">
         <v>363.15</v>
       </c>
@@ -1308,10 +1309,10 @@
         <v>0.2346</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="14">
         <v>363.15</v>
       </c>
@@ -1322,10 +1323,10 @@
         <v>0.2104</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="14">
         <v>363.15</v>
       </c>
@@ -1336,10 +1337,10 @@
         <v>0.188</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="14">
         <v>363.15</v>
       </c>
@@ -1350,10 +1351,10 @@
         <v>0.1643</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="14">
         <v>363.15</v>
       </c>
@@ -1364,10 +1365,10 @@
         <v>0.1416</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="14">
         <v>363.15</v>
       </c>
@@ -1378,10 +1379,10 @@
         <v>0.1196</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="14">
         <v>363.15</v>
       </c>
@@ -1392,10 +1393,10 @@
         <v>9.9000000000000005E-2</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="14">
         <v>363.15</v>
       </c>
@@ -1406,10 +1407,10 @@
         <v>8.1100000000000005E-2</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="14">
         <v>363.15</v>
       </c>
@@ -1420,10 +1421,10 @@
         <v>7.0699999999999999E-2</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" s="14">
         <v>363.15</v>
       </c>
@@ -1434,10 +1435,10 @@
         <v>6.3100000000000003E-2</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="14">
         <v>383.15</v>
       </c>
@@ -1448,10 +1449,10 @@
         <v>0.28139999999999998</v>
       </c>
       <c r="D52" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="14">
         <v>383.15</v>
       </c>
@@ -1462,7 +1463,7 @@
         <v>0.2712</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>